<commit_message>
Demo Download Poll Excel Changes
</commit_message>
<xml_diff>
--- a/public/poll_sample.xlsx
+++ b/public/poll_sample.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Question</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>Test Question 3</t>
+  </si>
+  <si>
+    <t>Textbox</t>
   </si>
 </sst>
 </file>
@@ -152,11 +158,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -177,104 +183,116 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>